<commit_message>
Updated BOM to reflect 1206 chip components
</commit_message>
<xml_diff>
--- a/DugganPhilpLarsen BOM CC3501.xlsx
+++ b/DugganPhilpLarsen BOM CC3501.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aphil\Downloads\CC3501-Assignment-master (1)\CC3501-Assignment-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aphil\OneDrive\Desktop\New folder\CC3501-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389C0C6-205F-422B-9575-7AE9057C0FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6F4DD-C164-432A-BADB-1F19BA9D2CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Resistor 4.7k</t>
   </si>
   <si>
-    <t>MBR120VLSFT1G Schottky Rectifier, 20V, 1A</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -161,12 +158,6 @@
     <t>https://au.element14.com/te-connectivity/796136-1/assy-smt-battery-conn/dp/2775806?ost=796136-1</t>
   </si>
   <si>
-    <t>100nF chip</t>
-  </si>
-  <si>
-    <t>06035C222KAT2A 2.2nF chip</t>
-  </si>
-  <si>
     <t>Headers</t>
   </si>
   <si>
@@ -182,22 +173,31 @@
     <t>3.3V 800mA out</t>
   </si>
   <si>
-    <t>1uF chip 0805</t>
-  </si>
-  <si>
-    <t>10nF chip 0805</t>
-  </si>
-  <si>
-    <t>4.7k Ohms chip 0805</t>
-  </si>
-  <si>
-    <t>10k Ohms chip 0805</t>
-  </si>
-  <si>
-    <t>0 Ohm Resistor chip 0805</t>
-  </si>
-  <si>
-    <t>22pF chip 0805</t>
+    <t>100nF chip 1206</t>
+  </si>
+  <si>
+    <t>10nF chip 1206</t>
+  </si>
+  <si>
+    <t>1uF chip 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.2nF chip 1206</t>
+  </si>
+  <si>
+    <t>10k Ohms chip 1206</t>
+  </si>
+  <si>
+    <t>4.7k Ohms chip 1206</t>
+  </si>
+  <si>
+    <t>MBR120VLSFT1G Schottky Rectifier, 20V, 1A THD</t>
+  </si>
+  <si>
+    <t>0 Ohm Resistor chip 1206</t>
+  </si>
+  <si>
+    <t>22pF chip 1206</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -882,7 +882,7 @@
     </row>
     <row r="9" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -945,16 +945,16 @@
     </row>
     <row r="11" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1">
         <v>243308001</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="6">
         <v>3.17</v>
@@ -967,7 +967,7 @@
         <v>6.34</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -981,16 +981,16 @@
     </row>
     <row r="12" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>2377757</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="6">
         <v>2.72</v>
@@ -1003,7 +1003,7 @@
         <v>5.44</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="13" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1049,16 +1049,16 @@
     </row>
     <row r="14" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
         <v>2434224</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="6">
         <v>12.51</v>
@@ -1067,11 +1067,11 @@
         <v>2</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" ref="G14:G20" si="1">F14*E14</f>
+        <f t="shared" ref="G14:G19" si="1">F14*E14</f>
         <v>25.02</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="15" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1117,16 +1117,16 @@
     </row>
     <row r="16" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
         <v>2467817</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="6">
         <v>1.74</v>
@@ -1139,7 +1139,7 @@
         <v>3.48</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1153,16 +1153,16 @@
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <v>2775806</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="6">
         <v>4.66</v>
@@ -1175,7 +1175,7 @@
         <v>9.32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="18" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="19" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1253,16 +1253,16 @@
     </row>
     <row r="20" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
         <v>1652330</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E20" s="6">
         <v>1.27</v>
@@ -1275,7 +1275,7 @@
         <v>2.54</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>

</xml_diff>

<commit_message>
Fix remaining floating pins
</commit_message>
<xml_diff>
--- a/DugganPhilpLarsen BOM CC3501.xlsx
+++ b/DugganPhilpLarsen BOM CC3501.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aphil\OneDrive\Desktop\New folder\CC3501-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0f176aa6e24afd6/Engineering/2020 Semester 2/CC3501/CC3501-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6F4DD-C164-432A-BADB-1F19BA9D2CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9AC6F4DD-C164-432A-BADB-1F19BA9D2CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FFE7991-7254-46AA-8D1F-47512091D18F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1485" windowWidth="20445" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="57.85546875" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Correct cap value in BOM and clean up file structure
</commit_message>
<xml_diff>
--- a/DugganPhilpLarsen BOM CC3501.xlsx
+++ b/DugganPhilpLarsen BOM CC3501.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0f176aa6e24afd6/Engineering/2020 Semester 2/CC3501/CC3501-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9AC6F4DD-C164-432A-BADB-1F19BA9D2CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FFE7991-7254-46AA-8D1F-47512091D18F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9AC6F4DD-C164-432A-BADB-1F19BA9D2CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08CC5818-7641-4555-8CC7-36B25406C923}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1485" windowWidth="20445" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="885" windowWidth="20445" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Capacitor 1uF</t>
   </si>
   <si>
-    <t>Capacitor 2.2nF 50V</t>
-  </si>
-  <si>
     <t>Resistor 10k</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>22pF chip 1206</t>
+  </si>
+  <si>
+    <t>Capacitor 22pF 50V</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -789,7 +789,7 @@
     </row>
     <row r="6" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -820,7 +820,7 @@
     </row>
     <row r="7" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -851,7 +851,7 @@
     </row>
     <row r="8" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -882,7 +882,7 @@
     </row>
     <row r="9" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -945,16 +945,16 @@
     </row>
     <row r="11" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1">
         <v>243308001</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="6">
         <v>3.17</v>
@@ -967,7 +967,7 @@
         <v>6.34</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -981,16 +981,16 @@
     </row>
     <row r="12" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>2377757</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="6">
         <v>2.72</v>
@@ -1003,7 +1003,7 @@
         <v>5.44</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="13" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1049,16 +1049,16 @@
     </row>
     <row r="14" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <v>2434224</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6">
         <v>12.51</v>
@@ -1071,7 +1071,7 @@
         <v>25.02</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="15" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1117,16 +1117,16 @@
     </row>
     <row r="16" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>2467817</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="6">
         <v>1.74</v>
@@ -1139,7 +1139,7 @@
         <v>3.48</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1153,16 +1153,16 @@
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1">
         <v>2775806</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="6">
         <v>4.66</v>
@@ -1175,7 +1175,7 @@
         <v>9.32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="18" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="19" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1239,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1253,16 +1253,16 @@
     </row>
     <row r="20" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
         <v>1652330</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="6">
         <v>1.27</v>
@@ -1275,7 +1275,7 @@
         <v>2.54</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>

</xml_diff>